<commit_message>
njesite done kati 1
</commit_message>
<xml_diff>
--- a/706-3-Slivove-Asllani-leg/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës-706-3-Slivove-Asllani-leg.xlsx
+++ b/706-3-Slivove-Asllani-leg/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës-706-3-Slivove-Asllani-leg.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$127</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="21">
   <si>
     <t>Nr</t>
   </si>
@@ -585,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -776,6 +776,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -973,7 +976,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Zona Kadastrale: Greme</a:t>
+            <a:t>Zona Kadastrale: Slivovë</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1048,7 +1051,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>: 00173-4</a:t>
+            <a:t>: 00706-3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1077,6 +1080,325 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4586737" y="2598311"/>
+          <a:ext cx="3051603" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Sistemi koordinat: KosovaRef01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>451310</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>16719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4496634" y="207219"/>
+          <a:ext cx="850252" cy="669082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2975170" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1216804" y="2321550"/>
+          <a:ext cx="2975170" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Komuna: Ferizaj</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>839686</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>43127</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2953749" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4885010" y="2351539"/>
+          <a:ext cx="2953749" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Zona Kadastrale: Slivovë</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>606643</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>89338</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3298607" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1211761" y="2588250"/>
+          <a:ext cx="3298607" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Numri</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> i njësis kadastrale</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>: 00706-3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>842998</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>105246</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3051603" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4888322" y="2604158"/>
           <a:ext cx="3051603" cy="298800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1416,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="C31:H51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79:H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2655,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="J52" s="1"/>
@@ -2342,515 +2664,955 @@
     <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>3</v>
-      </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="5">
-        <v>25</v>
-      </c>
-      <c r="D54" s="4">
-        <v>7512908.7709999997</v>
-      </c>
-      <c r="E54" s="4">
-        <v>4688190.2439999999</v>
-      </c>
-      <c r="F54" s="70">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="G54" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="5">
-        <v>26</v>
-      </c>
-      <c r="D55" s="4">
-        <v>7512912.8032999998</v>
-      </c>
-      <c r="E55" s="4">
-        <v>4688202.5635000002</v>
-      </c>
-      <c r="F55" s="70"/>
-      <c r="G55" s="70"/>
-      <c r="H55" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="5">
-        <v>27</v>
-      </c>
-      <c r="D56" s="4">
-        <v>7512912.7340000002</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4688191.807</v>
-      </c>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
-      <c r="H56" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="5">
-        <v>28</v>
-      </c>
-      <c r="D57" s="4">
-        <v>7512912.3449999997</v>
-      </c>
-      <c r="E57" s="4">
-        <v>4688192.7699999996</v>
-      </c>
-      <c r="F57" s="70"/>
-      <c r="G57" s="70"/>
-      <c r="H57" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="5">
-        <v>29</v>
-      </c>
-      <c r="D58" s="4">
-        <v>7512908.3671000004</v>
-      </c>
-      <c r="E58" s="4">
-        <v>4688191.2390000001</v>
-      </c>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
-      <c r="H58" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="5">
-        <v>30</v>
-      </c>
-      <c r="D59" s="4">
-        <v>7512905.0429999996</v>
-      </c>
-      <c r="E59" s="4">
-        <v>4688199.4000000004</v>
-      </c>
-      <c r="F59" s="70"/>
-      <c r="G59" s="70"/>
-      <c r="H59" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="5">
-        <v>31</v>
-      </c>
-      <c r="D60" s="4">
-        <v>7512916.5610999996</v>
-      </c>
-      <c r="E60" s="4">
-        <v>4688193.3693000004</v>
-      </c>
-      <c r="F60" s="70"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="5">
-        <v>187</v>
-      </c>
-      <c r="D61" s="4">
-        <v>7512910.7204999998</v>
-      </c>
-      <c r="E61" s="4">
-        <v>4688201.7122999998</v>
-      </c>
-      <c r="F61" s="70"/>
-      <c r="G61" s="70"/>
-      <c r="H61" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="5">
-        <v>188</v>
-      </c>
-      <c r="D62" s="4">
-        <v>7512912.1381999999</v>
-      </c>
-      <c r="E62" s="4">
-        <v>4688198.2437000005</v>
-      </c>
-      <c r="F62" s="70"/>
-      <c r="G62" s="70"/>
-      <c r="H62" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="5">
-        <v>189</v>
-      </c>
-      <c r="D63" s="4">
-        <v>7512910.7767000003</v>
-      </c>
-      <c r="E63" s="4">
-        <v>4688197.6892999997</v>
-      </c>
-      <c r="F63" s="70"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="5">
-        <v>190</v>
-      </c>
-      <c r="D64" s="4">
-        <v>7512911.5334000001</v>
-      </c>
-      <c r="E64" s="4">
-        <v>4688195.8380000005</v>
-      </c>
-      <c r="F64" s="70"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
     <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="5">
-        <v>191</v>
-      </c>
-      <c r="D65" s="4">
-        <v>7512914.9718000004</v>
-      </c>
-      <c r="E65" s="4">
-        <v>4688197.2380999997</v>
-      </c>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
+      <c r="A65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="41"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" s="44"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="57"/>
     </row>
     <row r="66" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="6">
-        <v>181</v>
-      </c>
-      <c r="D66" s="7">
-        <v>7512913.2540999996</v>
-      </c>
-      <c r="E66" s="7">
-        <v>4688193.8757999996</v>
-      </c>
-      <c r="F66" s="71"/>
-      <c r="G66" s="71"/>
-      <c r="H66" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
+      <c r="A66" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="63">
+        <v>140</v>
+      </c>
+      <c r="F66" s="64"/>
+      <c r="G66" s="65"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="58"/>
+      <c r="K66" s="59"/>
     </row>
     <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="26"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-    </row>
-    <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-    </row>
-    <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-    </row>
-    <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-    </row>
-    <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-    </row>
-    <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-    </row>
-    <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
-      <c r="H75" s="25"/>
-      <c r="I75" s="25"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-    </row>
-    <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
-      <c r="I76" s="25"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
+    </row>
+    <row r="69" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="38"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="66"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="66"/>
+      <c r="B71" s="66"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="66"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="66"/>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="66"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="66"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="47"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="48"/>
+      <c r="I75" s="49"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="50"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="52"/>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="53"/>
+      <c r="D77" s="54"/>
+      <c r="E77" s="54"/>
+      <c r="F77" s="54"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="54"/>
+      <c r="I77" s="55"/>
     </row>
     <row r="78" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
-      <c r="I78" s="25"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="5">
+        <v>326</v>
+      </c>
+      <c r="D80" s="4">
+        <v>7508332.8404000001</v>
+      </c>
+      <c r="E80" s="4">
+        <v>4696776.3962000003</v>
+      </c>
+      <c r="F80" s="70">
+        <v>609.58299999999997</v>
+      </c>
+      <c r="G80" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="5">
+        <v>328</v>
+      </c>
+      <c r="D81" s="4">
+        <v>7508329.9861000003</v>
+      </c>
+      <c r="E81" s="4">
+        <v>4696771.2389000002</v>
+      </c>
+      <c r="F81" s="70"/>
+      <c r="G81" s="70"/>
+      <c r="H81" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="5">
+        <v>329</v>
+      </c>
+      <c r="D82" s="4">
+        <v>7508330.3726000004</v>
+      </c>
+      <c r="E82" s="4">
+        <v>4696773.2703</v>
+      </c>
+      <c r="F82" s="70"/>
+      <c r="G82" s="70"/>
+      <c r="H82" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="5">
+        <v>330</v>
+      </c>
+      <c r="D83" s="4">
+        <v>7508328.6403999999</v>
+      </c>
+      <c r="E83" s="4">
+        <v>4696777.1953999996</v>
+      </c>
+      <c r="F83" s="70"/>
+      <c r="G83" s="70"/>
+      <c r="H83" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="5">
+        <v>14</v>
+      </c>
+      <c r="D84" s="4">
+        <v>7508327.4062999999</v>
+      </c>
+      <c r="E84" s="4">
+        <v>4696770.5133999996</v>
+      </c>
+      <c r="F84" s="70"/>
+      <c r="G84" s="70"/>
+      <c r="H84" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="5">
+        <v>13</v>
+      </c>
+      <c r="D85" s="4">
+        <v>7508327.6256999997</v>
+      </c>
+      <c r="E85" s="4">
+        <v>4696771.6880000001</v>
+      </c>
+      <c r="F85" s="70"/>
+      <c r="G85" s="70"/>
+      <c r="H85" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="5">
+        <v>18</v>
+      </c>
+      <c r="D86" s="4">
+        <v>7508329.2152000004</v>
+      </c>
+      <c r="E86" s="4">
+        <v>4696780.3870000001</v>
+      </c>
+      <c r="F86" s="70"/>
+      <c r="G86" s="70"/>
+      <c r="H86" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="5">
+        <v>19</v>
+      </c>
+      <c r="D87" s="4">
+        <v>7508338.3417999996</v>
+      </c>
+      <c r="E87" s="4">
+        <v>4696778.6058999998</v>
+      </c>
+      <c r="F87" s="70"/>
+      <c r="G87" s="70"/>
+      <c r="H87" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="5">
+        <v>22</v>
+      </c>
+      <c r="D88" s="4">
+        <v>7508327.5800999999</v>
+      </c>
+      <c r="E88" s="4">
+        <v>4696776.3726000004</v>
+      </c>
+      <c r="F88" s="70"/>
+      <c r="G88" s="70"/>
+      <c r="H88" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="5">
+        <v>23</v>
+      </c>
+      <c r="D89" s="4">
+        <v>7508327.1117000002</v>
+      </c>
+      <c r="E89" s="4">
+        <v>4696773.8236999996</v>
+      </c>
+      <c r="F89" s="70"/>
+      <c r="G89" s="70"/>
+      <c r="H89" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="5">
+        <v>26</v>
+      </c>
+      <c r="D90" s="4">
+        <v>7508327.9957999997</v>
+      </c>
+      <c r="E90" s="4">
+        <v>4696773.6736000003</v>
+      </c>
+      <c r="F90" s="70"/>
+      <c r="G90" s="70"/>
+      <c r="H90" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="5">
+        <v>28</v>
+      </c>
+      <c r="D91" s="4">
+        <v>7508328.4636000004</v>
+      </c>
+      <c r="E91" s="4">
+        <v>4696776.2134999996</v>
+      </c>
+      <c r="F91" s="70"/>
+      <c r="G91" s="70"/>
+      <c r="H91" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="32">
+        <v>29</v>
+      </c>
+      <c r="D92" s="33">
+        <v>7508331.7936000004</v>
+      </c>
+      <c r="E92" s="33">
+        <v>4696770.8948999997</v>
+      </c>
+      <c r="F92" s="72"/>
+      <c r="G92" s="72"/>
+      <c r="H92" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="32">
+        <v>30</v>
+      </c>
+      <c r="D93" s="33">
+        <v>7508332.2145999996</v>
+      </c>
+      <c r="E93" s="33">
+        <v>4696770.6380000003</v>
+      </c>
+      <c r="F93" s="72"/>
+      <c r="G93" s="72"/>
+      <c r="H93" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="32">
+        <v>31</v>
+      </c>
+      <c r="D94" s="33">
+        <v>7508333.1083000004</v>
+      </c>
+      <c r="E94" s="33">
+        <v>4696769.4139</v>
+      </c>
+      <c r="F94" s="72"/>
+      <c r="G94" s="72"/>
+      <c r="H94" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="32">
+        <v>32</v>
+      </c>
+      <c r="D95" s="33">
+        <v>7508334.9506000001</v>
+      </c>
+      <c r="E95" s="33">
+        <v>4696769.0147000002</v>
+      </c>
+      <c r="F95" s="72"/>
+      <c r="G95" s="72"/>
+      <c r="H95" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="32">
+        <v>33</v>
+      </c>
+      <c r="D96" s="33">
+        <v>7508336.3622000003</v>
+      </c>
+      <c r="E96" s="33">
+        <v>4696769.9818000002</v>
+      </c>
+      <c r="F96" s="72"/>
+      <c r="G96" s="72"/>
+      <c r="H96" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
+    <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="32">
+        <v>34</v>
+      </c>
+      <c r="D97" s="33">
+        <v>7508336.6776999999</v>
+      </c>
+      <c r="E97" s="33">
+        <v>4696769.9379000003</v>
+      </c>
+      <c r="F97" s="72"/>
+      <c r="G97" s="72"/>
+      <c r="H97" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="6">
+        <v>325</v>
+      </c>
+      <c r="D98" s="7">
+        <v>7508331.0077</v>
+      </c>
+      <c r="E98" s="7">
+        <v>4696771.0444999998</v>
+      </c>
+      <c r="F98" s="71"/>
+      <c r="G98" s="71"/>
+      <c r="H98" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+    </row>
+    <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+    <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+    </row>
+    <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+    </row>
+    <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+    </row>
+    <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+    </row>
+    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+    </row>
+    <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="30"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="31"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="29"/>
+      <c r="D114" s="30"/>
+      <c r="E114" s="30"/>
+      <c r="F114" s="31"/>
+      <c r="G114" s="31"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="29"/>
+      <c r="D115" s="30"/>
+      <c r="E115" s="30"/>
+      <c r="F115" s="31"/>
+      <c r="G115" s="31"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="30"/>
+      <c r="F116" s="31"/>
+      <c r="G116" s="31"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="31"/>
+      <c r="G117" s="31"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="29"/>
+      <c r="D118" s="30"/>
+      <c r="E118" s="30"/>
+      <c r="F118" s="31"/>
+      <c r="G118" s="31"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="39"/>
+      <c r="I119" s="39"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="39"/>
+      <c r="D120" s="39"/>
+      <c r="E120" s="39"/>
+      <c r="F120" s="39"/>
+      <c r="G120" s="39"/>
+      <c r="H120" s="39"/>
+      <c r="I120" s="39"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="25"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+    </row>
+    <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="25"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="25"/>
+      <c r="H122" s="25"/>
+      <c r="I122" s="25"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="25"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="25"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="25"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="25"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="25"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="40" t="s">
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="43" t="s">
+      <c r="F125" s="41"/>
+      <c r="G125" s="42"/>
+      <c r="H125" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I79" s="44"/>
-      <c r="J79" s="56"/>
-      <c r="K79" s="57"/>
-    </row>
-    <row r="80" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="60" t="s">
+      <c r="I125" s="44"/>
+      <c r="J125" s="56"/>
+      <c r="K125" s="57"/>
+    </row>
+    <row r="126" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="61"/>
-      <c r="C80" s="61"/>
-      <c r="D80" s="62"/>
-      <c r="E80" s="63">
+      <c r="B126" s="61"/>
+      <c r="C126" s="61"/>
+      <c r="D126" s="62"/>
+      <c r="E126" s="63">
         <v>140</v>
       </c>
-      <c r="F80" s="64"/>
-      <c r="G80" s="65"/>
-      <c r="H80" s="45"/>
-      <c r="I80" s="46"/>
-      <c r="J80" s="58"/>
-      <c r="K80" s="59"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="38"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="38"/>
-      <c r="I81" s="38"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
+      <c r="F126" s="64"/>
+      <c r="G126" s="65"/>
+      <c r="H126" s="45"/>
+      <c r="I126" s="46"/>
+      <c r="J126" s="58"/>
+      <c r="K126" s="59"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="38"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="22">
     <mergeCell ref="A3:K6"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="F32:F51"/>
     <mergeCell ref="G32:G51"/>
-    <mergeCell ref="F54:F66"/>
-    <mergeCell ref="G54:G66"/>
-    <mergeCell ref="A81:K81"/>
-    <mergeCell ref="C73:I74"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H79:I80"/>
+    <mergeCell ref="F80:F98"/>
+    <mergeCell ref="G80:G98"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H65:I66"/>
+    <mergeCell ref="J65:K66"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="A68:K69"/>
+    <mergeCell ref="A70:K73"/>
+    <mergeCell ref="C75:I77"/>
+    <mergeCell ref="A127:K127"/>
+    <mergeCell ref="C119:I120"/>
+    <mergeCell ref="E125:G125"/>
+    <mergeCell ref="H125:I126"/>
     <mergeCell ref="C8:I10"/>
-    <mergeCell ref="J79:K80"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="J125:K126"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="E126:G126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>